<commit_message>
adding study 2 demo table
</commit_message>
<xml_diff>
--- a/data/m@hr/demo_table.xlsx
+++ b/data/m@hr/demo_table.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kathios.n/Documents/Research/TEAM/data/m@hr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B97561-72CC-6440-B615-D34DCDFC0201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF96D529-1614-E543-8A6C-C32A73B38A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{98B4B565-8E7C-2141-98CC-B5F89BB3EDF5}"/>
+    <workbookView xWindow="23320" yWindow="2420" windowWidth="28040" windowHeight="17440" xr2:uid="{98B4B565-8E7C-2141-98CC-B5F89BB3EDF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>Demographic</t>
   </si>
@@ -140,13 +140,40 @@
   </si>
   <si>
     <t>4 (1.39%)</t>
+  </si>
+  <si>
+    <t>30 (65.22%)</t>
+  </si>
+  <si>
+    <t>4 (8.7%)</t>
+  </si>
+  <si>
+    <t>0 (0%)</t>
+  </si>
+  <si>
+    <t>3 (6.52%)</t>
+  </si>
+  <si>
+    <t>196 (68.06%)</t>
+  </si>
+  <si>
+    <t>22 (7.64%)</t>
+  </si>
+  <si>
+    <t>16 (5.56%)</t>
+  </si>
+  <si>
+    <t>25 (8.68%)</t>
+  </si>
+  <si>
+    <t>27 (9.38)%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -166,6 +193,11 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times Roman"/>
     </font>
   </fonts>
   <fills count="2">
@@ -188,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -200,7 +232,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,37 +552,37 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
+    <row r="2" spans="1:3">
+      <c r="A2" s="7"/>
       <c r="B2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
@@ -559,14 +593,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -577,8 +611,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -588,8 +622,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -599,12 +633,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -615,7 +649,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -626,7 +660,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -637,7 +671,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -648,97 +682,97 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="2">
-        <v>0.68600000000000005</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0.6522</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="2">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="C15" s="2">
-        <v>8.6999999999999994E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="2">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="2">
-        <v>7.4399999999999994E-2</v>
-      </c>
-      <c r="C17" s="2">
-        <v>8.6999999999999994E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="2">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="2">
-        <v>5.3699999999999998E-2</v>
-      </c>
-      <c r="C19" s="2">
-        <v>6.5199999999999994E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="2">
-        <v>8.6800000000000002E-2</v>
-      </c>
-      <c r="C20" s="2">
-        <v>8.6999999999999994E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="2">
-        <v>4.1000000000000003E-3</v>
-      </c>
-      <c r="C21" s="2">
-        <v>2.1700000000000001E-2</v>
+      <c r="B21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>